<commit_message>
Restructuration of transitions matrix.
</commit_message>
<xml_diff>
--- a/lexic/transitionsDescription.xlsx
+++ b/lexic/transitionsDescription.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="42">
   <si>
     <t>estado</t>
   </si>
@@ -130,14 +130,34 @@
   </si>
   <si>
     <t>ER</t>
+  </si>
+  <si>
+    <t>PR01</t>
+  </si>
+  <si>
+    <t>incluir</t>
+  </si>
+  <si>
+    <t>PR02</t>
+  </si>
+  <si>
+    <t>principal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -171,10 +191,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AO37"/>
+  <dimension ref="A2:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AM18" sqref="AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -785,11 +806,11 @@
       <c r="E9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>37</v>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>37</v>
@@ -819,7 +840,7 @@
         <v>37</v>
       </c>
       <c r="Q9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R9" t="s">
         <v>37</v>
@@ -827,8 +848,8 @@
       <c r="S9" t="s">
         <v>37</v>
       </c>
-      <c r="T9" t="s">
-        <v>37</v>
+      <c r="T9">
+        <v>41</v>
       </c>
       <c r="U9" t="s">
         <v>37</v>
@@ -887,8 +908,8 @@
       <c r="AM9" t="s">
         <v>37</v>
       </c>
-      <c r="AN9" t="s">
-        <v>37</v>
+      <c r="AN9">
+        <v>1</v>
       </c>
       <c r="AO9" t="s">
         <v>37</v>
@@ -910,11 +931,11 @@
       <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>28</v>
       </c>
       <c r="H10" t="s">
         <v>37</v>
@@ -944,7 +965,7 @@
         <v>37</v>
       </c>
       <c r="Q10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R10" t="s">
         <v>37</v>
@@ -952,8 +973,8 @@
       <c r="S10" t="s">
         <v>37</v>
       </c>
-      <c r="T10" t="s">
-        <v>37</v>
+      <c r="T10">
+        <v>41</v>
       </c>
       <c r="U10" t="s">
         <v>37</v>
@@ -1006,14 +1027,14 @@
       <c r="AK10" t="s">
         <v>37</v>
       </c>
-      <c r="AL10" t="s">
-        <v>37</v>
+      <c r="AL10">
+        <v>1</v>
       </c>
       <c r="AM10" t="s">
         <v>37</v>
       </c>
-      <c r="AN10" t="s">
-        <v>37</v>
+      <c r="AN10">
+        <v>1</v>
       </c>
       <c r="AO10" t="s">
         <v>37</v>
@@ -1769,7 +1790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:43">
       <c r="A17" s="2">
         <v>8</v>
       </c>
@@ -1881,20 +1902,20 @@
       <c r="AK17" t="s">
         <v>37</v>
       </c>
-      <c r="AL17" t="s">
-        <v>37</v>
+      <c r="AL17">
+        <v>9</v>
       </c>
       <c r="AM17" t="s">
         <v>37</v>
       </c>
-      <c r="AN17" t="s">
-        <v>37</v>
+      <c r="AN17">
+        <v>9</v>
       </c>
       <c r="AO17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:43">
       <c r="A18" s="2">
         <v>9</v>
       </c>
@@ -1949,8 +1970,8 @@
       <c r="R18" t="s">
         <v>37</v>
       </c>
-      <c r="S18">
-        <v>10</v>
+      <c r="S18" t="s">
+        <v>37</v>
       </c>
       <c r="T18" t="s">
         <v>37</v>
@@ -2009,7 +2030,7 @@
       <c r="AL18" t="s">
         <v>37</v>
       </c>
-      <c r="AM18" t="s">
+      <c r="AM18" s="3" t="s">
         <v>37</v>
       </c>
       <c r="AN18" t="s">
@@ -2018,8 +2039,14 @@
       <c r="AO18" t="s">
         <v>37</v>
       </c>
+      <c r="AP18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:43">
       <c r="A19" s="2">
         <v>10</v>
       </c>
@@ -2047,36 +2074,36 @@
       <c r="I19" t="s">
         <v>37</v>
       </c>
-      <c r="J19">
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O19" t="s">
+        <v>37</v>
+      </c>
+      <c r="P19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19">
         <v>11</v>
       </c>
-      <c r="K19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L19" t="s">
-        <v>37</v>
-      </c>
-      <c r="M19" t="s">
-        <v>37</v>
-      </c>
-      <c r="N19" t="s">
-        <v>37</v>
-      </c>
-      <c r="O19" t="s">
-        <v>37</v>
-      </c>
-      <c r="P19" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>37</v>
-      </c>
-      <c r="R19" t="s">
-        <v>37</v>
-      </c>
-      <c r="S19" t="s">
-        <v>37</v>
-      </c>
       <c r="T19" t="s">
         <v>37</v>
       </c>
@@ -2144,7 +2171,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:41">
+    <row r="20" spans="1:43">
       <c r="A20" s="2">
         <v>11</v>
       </c>
@@ -2172,8 +2199,8 @@
       <c r="I20" t="s">
         <v>37</v>
       </c>
-      <c r="J20" t="s">
-        <v>37</v>
+      <c r="J20">
+        <v>12</v>
       </c>
       <c r="K20" t="s">
         <v>37</v>
@@ -2187,8 +2214,8 @@
       <c r="N20" t="s">
         <v>37</v>
       </c>
-      <c r="O20">
-        <v>12</v>
+      <c r="O20" t="s">
+        <v>37</v>
       </c>
       <c r="P20" t="s">
         <v>37</v>
@@ -2269,7 +2296,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:41">
+    <row r="21" spans="1:43">
       <c r="A21" s="2">
         <v>12</v>
       </c>
@@ -2279,42 +2306,42 @@
       <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" t="s">
-        <v>37</v>
-      </c>
-      <c r="L21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N21" t="s">
-        <v>37</v>
-      </c>
-      <c r="O21" t="s">
-        <v>37</v>
-      </c>
       <c r="P21" t="s">
         <v>37</v>
       </c>
@@ -2394,7 +2421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:41">
+    <row r="22" spans="1:43">
       <c r="A22" s="2">
         <v>13</v>
       </c>
@@ -2404,8 +2431,8 @@
       <c r="C22" t="s">
         <v>37</v>
       </c>
-      <c r="D22" t="s">
-        <v>37</v>
+      <c r="D22">
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
@@ -2422,8 +2449,8 @@
       <c r="I22" t="s">
         <v>37</v>
       </c>
-      <c r="J22">
-        <v>14</v>
+      <c r="J22" t="s">
+        <v>37</v>
       </c>
       <c r="K22" t="s">
         <v>37</v>
@@ -2519,7 +2546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:41">
+    <row r="23" spans="1:43">
       <c r="A23" s="2">
         <v>14</v>
       </c>
@@ -2547,8 +2574,8 @@
       <c r="I23" t="s">
         <v>37</v>
       </c>
-      <c r="J23" t="s">
-        <v>37</v>
+      <c r="J23">
+        <v>15</v>
       </c>
       <c r="K23" t="s">
         <v>37</v>
@@ -2568,8 +2595,8 @@
       <c r="P23" t="s">
         <v>37</v>
       </c>
-      <c r="Q23">
-        <v>15</v>
+      <c r="Q23" t="s">
+        <v>37</v>
       </c>
       <c r="R23" t="s">
         <v>37</v>
@@ -2644,58 +2671,58 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:41">
+    <row r="24" spans="1:43">
       <c r="A24" s="2">
         <v>15</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24" t="s">
+        <v>37</v>
+      </c>
+      <c r="P24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q24">
         <v>16</v>
       </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I24" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" t="s">
-        <v>37</v>
-      </c>
-      <c r="L24" t="s">
-        <v>37</v>
-      </c>
-      <c r="M24" t="s">
-        <v>37</v>
-      </c>
-      <c r="N24" t="s">
-        <v>37</v>
-      </c>
-      <c r="O24" t="s">
-        <v>37</v>
-      </c>
-      <c r="P24" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>37</v>
-      </c>
       <c r="R24" t="s">
         <v>37</v>
       </c>
@@ -2769,12 +2796,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:41">
+    <row r="25" spans="1:43">
       <c r="A25" s="2">
         <v>16</v>
       </c>
-      <c r="B25" t="s">
-        <v>37</v>
+      <c r="B25">
+        <v>17</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
@@ -2806,8 +2833,8 @@
       <c r="L25" t="s">
         <v>37</v>
       </c>
-      <c r="M25">
-        <v>17</v>
+      <c r="M25" t="s">
+        <v>37</v>
       </c>
       <c r="N25" t="s">
         <v>37</v>
@@ -2894,7 +2921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:41">
+    <row r="26" spans="1:43">
       <c r="A26" s="2">
         <v>17</v>
       </c>
@@ -2931,8 +2958,8 @@
       <c r="L26" t="s">
         <v>37</v>
       </c>
-      <c r="M26" t="s">
-        <v>37</v>
+      <c r="M26">
+        <v>18</v>
       </c>
       <c r="N26" t="s">
         <v>37</v>
@@ -3019,27 +3046,273 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:41">
+    <row r="27" spans="1:43">
       <c r="A27" s="2">
         <v>18</v>
       </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R27" t="s">
+        <v>37</v>
+      </c>
+      <c r="S27" t="s">
+        <v>37</v>
+      </c>
+      <c r="T27" t="s">
+        <v>37</v>
+      </c>
+      <c r="U27" t="s">
+        <v>37</v>
+      </c>
+      <c r="V27" t="s">
+        <v>37</v>
+      </c>
+      <c r="W27" t="s">
+        <v>37</v>
+      </c>
+      <c r="X27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL27">
+        <v>19</v>
+      </c>
+      <c r="AM27">
+        <v>19</v>
+      </c>
+      <c r="AN27">
+        <v>19</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:43">
       <c r="A28" s="2">
         <v>19</v>
       </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M28" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" t="s">
+        <v>37</v>
+      </c>
+      <c r="P28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>37</v>
+      </c>
+      <c r="R28" t="s">
+        <v>37</v>
+      </c>
+      <c r="S28" t="s">
+        <v>37</v>
+      </c>
+      <c r="T28" t="s">
+        <v>37</v>
+      </c>
+      <c r="U28" t="s">
+        <v>37</v>
+      </c>
+      <c r="V28" t="s">
+        <v>37</v>
+      </c>
+      <c r="W28" t="s">
+        <v>37</v>
+      </c>
+      <c r="X28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="29" spans="1:41">
+    <row r="29" spans="1:43">
       <c r="A29" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:41">
+    <row r="30" spans="1:43">
       <c r="A30" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:41">
+    <row r="31" spans="1:43">
       <c r="A31" s="2">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Addition of word 'escribe'.
</commit_message>
<xml_diff>
--- a/lexic/transitionsDescription.xlsx
+++ b/lexic/transitionsDescription.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="44">
   <si>
     <t>estado</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>principal</t>
+  </si>
+  <si>
+    <t>PR03</t>
+  </si>
+  <si>
+    <t>escribe</t>
   </si>
 </sst>
 </file>
@@ -492,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AM18" sqref="AM18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AP41" sqref="AP41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3306,18 +3312,1009 @@
       <c r="A29" s="2">
         <v>20</v>
       </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M29" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O29" t="s">
+        <v>37</v>
+      </c>
+      <c r="P29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>37</v>
+      </c>
+      <c r="R29" t="s">
+        <v>37</v>
+      </c>
+      <c r="S29" t="s">
+        <v>37</v>
+      </c>
+      <c r="T29">
+        <v>21</v>
+      </c>
+      <c r="U29" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29" t="s">
+        <v>37</v>
+      </c>
+      <c r="W29" t="s">
+        <v>37</v>
+      </c>
+      <c r="X29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:43">
       <c r="A30" s="2">
         <v>21</v>
       </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" t="s">
+        <v>37</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+      <c r="N30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O30" t="s">
+        <v>37</v>
+      </c>
+      <c r="P30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>37</v>
+      </c>
+      <c r="R30" t="s">
+        <v>37</v>
+      </c>
+      <c r="S30" t="s">
+        <v>37</v>
+      </c>
+      <c r="T30" t="s">
+        <v>37</v>
+      </c>
+      <c r="U30" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" t="s">
+        <v>37</v>
+      </c>
+      <c r="W30" t="s">
+        <v>37</v>
+      </c>
+      <c r="X30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" spans="1:43">
       <c r="A31" s="2">
         <v>22</v>
       </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" t="s">
+        <v>37</v>
+      </c>
+      <c r="M31" t="s">
+        <v>37</v>
+      </c>
+      <c r="N31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>37</v>
+      </c>
+      <c r="R31" t="s">
+        <v>37</v>
+      </c>
+      <c r="S31">
+        <v>23</v>
+      </c>
+      <c r="T31" t="s">
+        <v>37</v>
+      </c>
+      <c r="U31" t="s">
+        <v>37</v>
+      </c>
+      <c r="V31" t="s">
+        <v>37</v>
+      </c>
+      <c r="W31" t="s">
+        <v>37</v>
+      </c>
+      <c r="X31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO31" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="32" spans="1:43">
+      <c r="A32" s="2">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32">
+        <v>24</v>
+      </c>
+      <c r="K32" t="s">
+        <v>37</v>
+      </c>
+      <c r="L32" t="s">
+        <v>37</v>
+      </c>
+      <c r="M32" t="s">
+        <v>37</v>
+      </c>
+      <c r="N32" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" t="s">
+        <v>37</v>
+      </c>
+      <c r="P32" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>37</v>
+      </c>
+      <c r="R32" t="s">
+        <v>37</v>
+      </c>
+      <c r="S32" t="s">
+        <v>37</v>
+      </c>
+      <c r="T32" t="s">
+        <v>37</v>
+      </c>
+      <c r="U32" t="s">
+        <v>37</v>
+      </c>
+      <c r="V32" t="s">
+        <v>37</v>
+      </c>
+      <c r="W32" t="s">
+        <v>37</v>
+      </c>
+      <c r="X32" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43">
+      <c r="A33" s="2">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="s">
+        <v>37</v>
+      </c>
+      <c r="L33" t="s">
+        <v>37</v>
+      </c>
+      <c r="M33" t="s">
+        <v>37</v>
+      </c>
+      <c r="N33" t="s">
+        <v>37</v>
+      </c>
+      <c r="O33" t="s">
+        <v>37</v>
+      </c>
+      <c r="P33" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>37</v>
+      </c>
+      <c r="R33" t="s">
+        <v>37</v>
+      </c>
+      <c r="S33" t="s">
+        <v>37</v>
+      </c>
+      <c r="T33" t="s">
+        <v>37</v>
+      </c>
+      <c r="U33" t="s">
+        <v>37</v>
+      </c>
+      <c r="V33" t="s">
+        <v>37</v>
+      </c>
+      <c r="W33" t="s">
+        <v>37</v>
+      </c>
+      <c r="X33" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43">
+      <c r="A34" s="2">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34">
+        <v>26</v>
+      </c>
+      <c r="G34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" t="s">
+        <v>37</v>
+      </c>
+      <c r="L34" t="s">
+        <v>37</v>
+      </c>
+      <c r="M34" t="s">
+        <v>37</v>
+      </c>
+      <c r="N34" t="s">
+        <v>37</v>
+      </c>
+      <c r="O34" t="s">
+        <v>37</v>
+      </c>
+      <c r="P34" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>37</v>
+      </c>
+      <c r="R34" t="s">
+        <v>37</v>
+      </c>
+      <c r="S34" t="s">
+        <v>37</v>
+      </c>
+      <c r="T34" t="s">
+        <v>37</v>
+      </c>
+      <c r="U34" t="s">
+        <v>37</v>
+      </c>
+      <c r="V34" t="s">
+        <v>37</v>
+      </c>
+      <c r="W34" t="s">
+        <v>37</v>
+      </c>
+      <c r="X34" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43">
+      <c r="A35" s="2">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" t="s">
+        <v>37</v>
+      </c>
+      <c r="L35" t="s">
+        <v>37</v>
+      </c>
+      <c r="M35" t="s">
+        <v>37</v>
+      </c>
+      <c r="N35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35" t="s">
+        <v>37</v>
+      </c>
+      <c r="P35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>37</v>
+      </c>
+      <c r="R35" t="s">
+        <v>37</v>
+      </c>
+      <c r="S35" t="s">
+        <v>37</v>
+      </c>
+      <c r="T35" t="s">
+        <v>37</v>
+      </c>
+      <c r="U35" t="s">
+        <v>37</v>
+      </c>
+      <c r="V35" t="s">
+        <v>37</v>
+      </c>
+      <c r="W35" t="s">
+        <v>37</v>
+      </c>
+      <c r="X35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL35">
+        <v>27</v>
+      </c>
+      <c r="AM35">
+        <v>27</v>
+      </c>
+      <c r="AN35">
+        <v>27</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43">
+      <c r="A36" s="2">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" t="s">
+        <v>37</v>
+      </c>
+      <c r="N36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O36" t="s">
+        <v>37</v>
+      </c>
+      <c r="P36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>37</v>
+      </c>
+      <c r="R36" t="s">
+        <v>37</v>
+      </c>
+      <c r="S36" t="s">
+        <v>37</v>
+      </c>
+      <c r="T36" t="s">
+        <v>37</v>
+      </c>
+      <c r="U36" t="s">
+        <v>37</v>
+      </c>
+      <c r="V36" t="s">
+        <v>37</v>
+      </c>
+      <c r="W36" t="s">
+        <v>37</v>
+      </c>
+      <c r="X36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP36" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:43">
       <c r="A37" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Addition of word 'finprincipal, si, sino'.
</commit_message>
<xml_diff>
--- a/lexic/transitionsDescription.xlsx
+++ b/lexic/transitionsDescription.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="48">
   <si>
     <t>estado</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>escribe</t>
+  </si>
+  <si>
+    <t>PR04</t>
+  </si>
+  <si>
+    <t>finprincipal</t>
+  </si>
+  <si>
+    <t>PR05</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
 </sst>
 </file>
@@ -496,10 +508,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AQ37"/>
+  <dimension ref="A2:AQ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AP41" sqref="AP41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4315,7 +4329,2344 @@
       </c>
     </row>
     <row r="37" spans="1:43">
-      <c r="A37" t="s">
+      <c r="A37" s="2">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37">
+        <v>29</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37" t="s">
+        <v>37</v>
+      </c>
+      <c r="N37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P37" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37" t="s">
+        <v>37</v>
+      </c>
+      <c r="S37" t="s">
+        <v>37</v>
+      </c>
+      <c r="T37" t="s">
+        <v>37</v>
+      </c>
+      <c r="U37" t="s">
+        <v>37</v>
+      </c>
+      <c r="V37" t="s">
+        <v>37</v>
+      </c>
+      <c r="W37" t="s">
+        <v>37</v>
+      </c>
+      <c r="X37" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43">
+      <c r="A38" s="2">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L38" t="s">
+        <v>37</v>
+      </c>
+      <c r="M38" t="s">
+        <v>37</v>
+      </c>
+      <c r="N38" t="s">
+        <v>37</v>
+      </c>
+      <c r="O38">
+        <v>30</v>
+      </c>
+      <c r="P38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>37</v>
+      </c>
+      <c r="R38" t="s">
+        <v>37</v>
+      </c>
+      <c r="S38" t="s">
+        <v>37</v>
+      </c>
+      <c r="T38" t="s">
+        <v>37</v>
+      </c>
+      <c r="U38" t="s">
+        <v>37</v>
+      </c>
+      <c r="V38" t="s">
+        <v>37</v>
+      </c>
+      <c r="W38" t="s">
+        <v>37</v>
+      </c>
+      <c r="X38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43">
+      <c r="A39" s="2">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" t="s">
+        <v>37</v>
+      </c>
+      <c r="L39" t="s">
+        <v>37</v>
+      </c>
+      <c r="M39" t="s">
+        <v>37</v>
+      </c>
+      <c r="N39" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39" t="s">
+        <v>37</v>
+      </c>
+      <c r="P39" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q39">
+        <v>31</v>
+      </c>
+      <c r="R39" t="s">
+        <v>37</v>
+      </c>
+      <c r="S39" t="s">
+        <v>37</v>
+      </c>
+      <c r="T39" t="s">
+        <v>37</v>
+      </c>
+      <c r="U39" t="s">
+        <v>37</v>
+      </c>
+      <c r="V39" t="s">
+        <v>37</v>
+      </c>
+      <c r="W39" t="s">
+        <v>37</v>
+      </c>
+      <c r="X39" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43">
+      <c r="A40" s="2">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40" t="s">
+        <v>37</v>
+      </c>
+      <c r="N40" t="s">
+        <v>37</v>
+      </c>
+      <c r="O40" t="s">
+        <v>37</v>
+      </c>
+      <c r="P40" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>37</v>
+      </c>
+      <c r="R40" t="s">
+        <v>37</v>
+      </c>
+      <c r="S40">
+        <v>32</v>
+      </c>
+      <c r="T40" t="s">
+        <v>37</v>
+      </c>
+      <c r="U40" t="s">
+        <v>37</v>
+      </c>
+      <c r="V40" t="s">
+        <v>37</v>
+      </c>
+      <c r="W40" t="s">
+        <v>37</v>
+      </c>
+      <c r="X40" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43">
+      <c r="A41" s="2">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+      <c r="J41">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" t="s">
+        <v>37</v>
+      </c>
+      <c r="M41" t="s">
+        <v>37</v>
+      </c>
+      <c r="N41" t="s">
+        <v>37</v>
+      </c>
+      <c r="O41" t="s">
+        <v>37</v>
+      </c>
+      <c r="P41" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>37</v>
+      </c>
+      <c r="R41" t="s">
+        <v>37</v>
+      </c>
+      <c r="S41" t="s">
+        <v>37</v>
+      </c>
+      <c r="T41" t="s">
+        <v>37</v>
+      </c>
+      <c r="U41" t="s">
+        <v>37</v>
+      </c>
+      <c r="V41" t="s">
+        <v>37</v>
+      </c>
+      <c r="W41" t="s">
+        <v>37</v>
+      </c>
+      <c r="X41" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:43">
+      <c r="A42" s="2">
+        <v>33</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" t="s">
+        <v>37</v>
+      </c>
+      <c r="G42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" t="s">
+        <v>37</v>
+      </c>
+      <c r="M42" t="s">
+        <v>37</v>
+      </c>
+      <c r="N42" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42">
+        <v>34</v>
+      </c>
+      <c r="P42" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>37</v>
+      </c>
+      <c r="R42" t="s">
+        <v>37</v>
+      </c>
+      <c r="S42" t="s">
+        <v>37</v>
+      </c>
+      <c r="T42" t="s">
+        <v>37</v>
+      </c>
+      <c r="U42" t="s">
+        <v>37</v>
+      </c>
+      <c r="V42" t="s">
+        <v>37</v>
+      </c>
+      <c r="W42" t="s">
+        <v>37</v>
+      </c>
+      <c r="X42" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:43">
+      <c r="A43" s="2">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43">
+        <v>35</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" t="s">
+        <v>37</v>
+      </c>
+      <c r="G43" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+      <c r="J43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" t="s">
+        <v>37</v>
+      </c>
+      <c r="M43" t="s">
+        <v>37</v>
+      </c>
+      <c r="N43" t="s">
+        <v>37</v>
+      </c>
+      <c r="O43" t="s">
+        <v>37</v>
+      </c>
+      <c r="P43" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>37</v>
+      </c>
+      <c r="R43" t="s">
+        <v>37</v>
+      </c>
+      <c r="S43" t="s">
+        <v>37</v>
+      </c>
+      <c r="T43" t="s">
+        <v>37</v>
+      </c>
+      <c r="U43" t="s">
+        <v>37</v>
+      </c>
+      <c r="V43" t="s">
+        <v>37</v>
+      </c>
+      <c r="W43" t="s">
+        <v>37</v>
+      </c>
+      <c r="X43" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43">
+      <c r="A44" s="2">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44">
+        <v>36</v>
+      </c>
+      <c r="K44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" t="s">
+        <v>37</v>
+      </c>
+      <c r="M44" t="s">
+        <v>37</v>
+      </c>
+      <c r="N44" t="s">
+        <v>37</v>
+      </c>
+      <c r="O44" t="s">
+        <v>37</v>
+      </c>
+      <c r="P44" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>37</v>
+      </c>
+      <c r="R44" t="s">
+        <v>37</v>
+      </c>
+      <c r="S44" t="s">
+        <v>37</v>
+      </c>
+      <c r="T44" t="s">
+        <v>37</v>
+      </c>
+      <c r="U44" t="s">
+        <v>37</v>
+      </c>
+      <c r="V44" t="s">
+        <v>37</v>
+      </c>
+      <c r="W44" t="s">
+        <v>37</v>
+      </c>
+      <c r="X44" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:43">
+      <c r="A45" s="2">
+        <v>36</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" t="s">
+        <v>37</v>
+      </c>
+      <c r="G45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" t="s">
+        <v>37</v>
+      </c>
+      <c r="M45" t="s">
+        <v>37</v>
+      </c>
+      <c r="N45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45" t="s">
+        <v>37</v>
+      </c>
+      <c r="P45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q45">
+        <v>37</v>
+      </c>
+      <c r="R45" t="s">
+        <v>37</v>
+      </c>
+      <c r="S45" t="s">
+        <v>37</v>
+      </c>
+      <c r="T45" t="s">
+        <v>37</v>
+      </c>
+      <c r="U45" t="s">
+        <v>37</v>
+      </c>
+      <c r="V45" t="s">
+        <v>37</v>
+      </c>
+      <c r="W45" t="s">
+        <v>37</v>
+      </c>
+      <c r="X45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:43">
+      <c r="A46" s="2">
+        <v>37</v>
+      </c>
+      <c r="B46">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" t="s">
+        <v>37</v>
+      </c>
+      <c r="H46" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" t="s">
+        <v>37</v>
+      </c>
+      <c r="J46" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" t="s">
+        <v>37</v>
+      </c>
+      <c r="M46" t="s">
+        <v>37</v>
+      </c>
+      <c r="N46" t="s">
+        <v>37</v>
+      </c>
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+      <c r="P46" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>37</v>
+      </c>
+      <c r="R46" t="s">
+        <v>37</v>
+      </c>
+      <c r="S46" t="s">
+        <v>37</v>
+      </c>
+      <c r="T46" t="s">
+        <v>37</v>
+      </c>
+      <c r="U46" t="s">
+        <v>37</v>
+      </c>
+      <c r="V46" t="s">
+        <v>37</v>
+      </c>
+      <c r="W46" t="s">
+        <v>37</v>
+      </c>
+      <c r="X46" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:43">
+      <c r="A47" s="2">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" t="s">
+        <v>37</v>
+      </c>
+      <c r="H47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47" t="s">
+        <v>37</v>
+      </c>
+      <c r="J47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" t="s">
+        <v>37</v>
+      </c>
+      <c r="L47" t="s">
+        <v>37</v>
+      </c>
+      <c r="M47">
+        <v>39</v>
+      </c>
+      <c r="N47" t="s">
+        <v>37</v>
+      </c>
+      <c r="O47" t="s">
+        <v>37</v>
+      </c>
+      <c r="P47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>37</v>
+      </c>
+      <c r="R47" t="s">
+        <v>37</v>
+      </c>
+      <c r="S47" t="s">
+        <v>37</v>
+      </c>
+      <c r="T47" t="s">
+        <v>37</v>
+      </c>
+      <c r="U47" t="s">
+        <v>37</v>
+      </c>
+      <c r="V47" t="s">
+        <v>37</v>
+      </c>
+      <c r="W47" t="s">
+        <v>37</v>
+      </c>
+      <c r="X47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43">
+      <c r="A48" s="2">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" t="s">
+        <v>37</v>
+      </c>
+      <c r="G48" t="s">
+        <v>37</v>
+      </c>
+      <c r="H48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48" t="s">
+        <v>37</v>
+      </c>
+      <c r="J48" t="s">
+        <v>37</v>
+      </c>
+      <c r="K48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L48" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48" t="s">
+        <v>37</v>
+      </c>
+      <c r="P48" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>37</v>
+      </c>
+      <c r="R48" t="s">
+        <v>37</v>
+      </c>
+      <c r="S48" t="s">
+        <v>37</v>
+      </c>
+      <c r="T48" t="s">
+        <v>37</v>
+      </c>
+      <c r="U48" t="s">
+        <v>37</v>
+      </c>
+      <c r="V48" t="s">
+        <v>37</v>
+      </c>
+      <c r="W48" t="s">
+        <v>37</v>
+      </c>
+      <c r="X48" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK48" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL48">
+        <v>40</v>
+      </c>
+      <c r="AM48">
+        <v>40</v>
+      </c>
+      <c r="AN48">
+        <v>40</v>
+      </c>
+      <c r="AO48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43">
+      <c r="A49" s="2">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+      <c r="G49" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" t="s">
+        <v>37</v>
+      </c>
+      <c r="J49" t="s">
+        <v>37</v>
+      </c>
+      <c r="K49" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M49" t="s">
+        <v>37</v>
+      </c>
+      <c r="N49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O49" t="s">
+        <v>37</v>
+      </c>
+      <c r="P49" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>37</v>
+      </c>
+      <c r="R49" t="s">
+        <v>37</v>
+      </c>
+      <c r="S49" t="s">
+        <v>37</v>
+      </c>
+      <c r="T49" t="s">
+        <v>37</v>
+      </c>
+      <c r="U49" t="s">
+        <v>37</v>
+      </c>
+      <c r="V49" t="s">
+        <v>37</v>
+      </c>
+      <c r="W49" t="s">
+        <v>37</v>
+      </c>
+      <c r="X49" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:43">
+      <c r="A50" s="2">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" t="s">
+        <v>37</v>
+      </c>
+      <c r="G50" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" t="s">
+        <v>37</v>
+      </c>
+      <c r="I50" t="s">
+        <v>37</v>
+      </c>
+      <c r="J50">
+        <v>42</v>
+      </c>
+      <c r="K50" t="s">
+        <v>37</v>
+      </c>
+      <c r="L50" t="s">
+        <v>37</v>
+      </c>
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" t="s">
+        <v>37</v>
+      </c>
+      <c r="O50" t="s">
+        <v>37</v>
+      </c>
+      <c r="P50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>37</v>
+      </c>
+      <c r="R50" t="s">
+        <v>37</v>
+      </c>
+      <c r="S50" t="s">
+        <v>37</v>
+      </c>
+      <c r="T50" t="s">
+        <v>37</v>
+      </c>
+      <c r="U50" t="s">
+        <v>37</v>
+      </c>
+      <c r="V50" t="s">
+        <v>37</v>
+      </c>
+      <c r="W50" t="s">
+        <v>37</v>
+      </c>
+      <c r="X50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:43">
+      <c r="A51" s="2">
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" t="s">
+        <v>37</v>
+      </c>
+      <c r="H51" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51" t="s">
+        <v>37</v>
+      </c>
+      <c r="M51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N51" t="s">
+        <v>37</v>
+      </c>
+      <c r="O51">
+        <v>44</v>
+      </c>
+      <c r="P51" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>37</v>
+      </c>
+      <c r="R51" t="s">
+        <v>37</v>
+      </c>
+      <c r="S51" t="s">
+        <v>37</v>
+      </c>
+      <c r="T51" t="s">
+        <v>37</v>
+      </c>
+      <c r="U51" t="s">
+        <v>37</v>
+      </c>
+      <c r="V51" t="s">
+        <v>37</v>
+      </c>
+      <c r="W51" t="s">
+        <v>37</v>
+      </c>
+      <c r="X51" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL51">
+        <v>43</v>
+      </c>
+      <c r="AM51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN51">
+        <v>43</v>
+      </c>
+      <c r="AO51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43">
+      <c r="A52" s="2">
+        <v>43</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" t="s">
+        <v>37</v>
+      </c>
+      <c r="H52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I52" t="s">
+        <v>37</v>
+      </c>
+      <c r="J52" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52" t="s">
+        <v>37</v>
+      </c>
+      <c r="L52" t="s">
+        <v>37</v>
+      </c>
+      <c r="M52" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" t="s">
+        <v>37</v>
+      </c>
+      <c r="O52" t="s">
+        <v>37</v>
+      </c>
+      <c r="P52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>37</v>
+      </c>
+      <c r="R52" t="s">
+        <v>37</v>
+      </c>
+      <c r="S52" t="s">
+        <v>37</v>
+      </c>
+      <c r="T52" t="s">
+        <v>37</v>
+      </c>
+      <c r="U52" t="s">
+        <v>37</v>
+      </c>
+      <c r="V52" t="s">
+        <v>37</v>
+      </c>
+      <c r="W52" t="s">
+        <v>37</v>
+      </c>
+      <c r="X52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP52" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:43">
+      <c r="A53" s="2">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G53" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" t="s">
+        <v>37</v>
+      </c>
+      <c r="J53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K53" t="s">
+        <v>37</v>
+      </c>
+      <c r="L53" t="s">
+        <v>37</v>
+      </c>
+      <c r="M53" t="s">
+        <v>37</v>
+      </c>
+      <c r="N53" t="s">
+        <v>37</v>
+      </c>
+      <c r="O53" t="s">
+        <v>37</v>
+      </c>
+      <c r="P53">
+        <v>45</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>37</v>
+      </c>
+      <c r="R53" t="s">
+        <v>37</v>
+      </c>
+      <c r="S53" t="s">
+        <v>37</v>
+      </c>
+      <c r="T53" t="s">
+        <v>37</v>
+      </c>
+      <c r="U53" t="s">
+        <v>37</v>
+      </c>
+      <c r="V53" t="s">
+        <v>37</v>
+      </c>
+      <c r="W53" t="s">
+        <v>37</v>
+      </c>
+      <c r="X53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43">
+      <c r="A54" s="2">
+        <v>45</v>
+      </c>
+      <c r="B54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" t="s">
+        <v>37</v>
+      </c>
+      <c r="H54" t="s">
+        <v>37</v>
+      </c>
+      <c r="I54" t="s">
+        <v>37</v>
+      </c>
+      <c r="J54" t="s">
+        <v>37</v>
+      </c>
+      <c r="K54" t="s">
+        <v>37</v>
+      </c>
+      <c r="L54" t="s">
+        <v>37</v>
+      </c>
+      <c r="M54" t="s">
+        <v>37</v>
+      </c>
+      <c r="N54" t="s">
+        <v>37</v>
+      </c>
+      <c r="O54" t="s">
+        <v>37</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>37</v>
+      </c>
+      <c r="R54" t="s">
+        <v>37</v>
+      </c>
+      <c r="S54" t="s">
+        <v>37</v>
+      </c>
+      <c r="T54" t="s">
+        <v>37</v>
+      </c>
+      <c r="U54" t="s">
+        <v>37</v>
+      </c>
+      <c r="V54" t="s">
+        <v>37</v>
+      </c>
+      <c r="W54" t="s">
+        <v>37</v>
+      </c>
+      <c r="X54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL54">
+        <v>46</v>
+      </c>
+      <c r="AM54">
+        <v>46</v>
+      </c>
+      <c r="AN54">
+        <v>46</v>
+      </c>
+      <c r="AO54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:43">
+      <c r="A55" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:43">
+      <c r="A56" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:43">
+      <c r="A57" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:43">
+      <c r="A58" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:43">
+      <c r="A59" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:43">
+      <c r="A60" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:43">
+      <c r="A61" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:43">
+      <c r="A62" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:43">
+      <c r="A63" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:43">
+      <c r="A64" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>